<commit_message>
Add vim entries: tab/splite window manipulation
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
   <si>
     <t>Lang</t>
   </si>
@@ -385,6 +385,36 @@
   </si>
   <si>
     <t>1G or gg</t>
+  </si>
+  <si>
+    <t>:sp / :vsp</t>
+  </si>
+  <si>
+    <t>Splite open / Vertical Splite Open</t>
+  </si>
+  <si>
+    <t>:tabnew {filename}</t>
+  </si>
+  <si>
+    <t>Tab open</t>
+  </si>
+  <si>
+    <t>Move among splites</t>
+  </si>
+  <si>
+    <t>Move among tabs</t>
+  </si>
+  <si>
+    <t>gt / gT</t>
+  </si>
+  <si>
+    <t>:tabs</t>
+  </si>
+  <si>
+    <t>Show all tabs</t>
+  </si>
+  <si>
+    <t>Ctrl W + hjkl</t>
   </si>
 </sst>
 </file>
@@ -432,15 +462,21 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -457,16 +493,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -768,17 +891,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1">
@@ -940,7 +1063,7 @@
       </c>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1060,69 +1183,76 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="A35" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="B36" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="B37" t="s">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="B38" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="B39" t="s">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="B40" t="s">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="B41" t="s">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="B42" t="s">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1159,6 +1289,46 @@
       </c>
       <c r="C46" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add vim entry: run bash cmd in vim
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>Lang</t>
   </si>
@@ -415,6 +415,19 @@
   </si>
   <si>
     <t>Ctrl W + hjkl</t>
+  </si>
+  <si>
+    <t>Run command</t>
+  </si>
+  <si>
+    <t>:! Echo…</t>
+  </si>
+  <si>
+    <t>Search and replace</t>
+  </si>
+  <si>
+    <t>:s/foo/bar/g
+:%s/foo/bar/g (do all)</t>
   </si>
 </sst>
 </file>
@@ -568,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -591,6 +604,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,17 +907,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1">
@@ -1329,6 +1345,22 @@
       </c>
       <c r="C51" s="1" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" ht="30">
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add git entry about supertab plugin util for git
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
   <si>
     <t>Lang</t>
   </si>
@@ -429,16 +429,47 @@
     <t>:s/foo/bar/g
 :%s/foo/bar/g (do all)</t>
   </si>
+  <si>
+    <t>git script</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Topic</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Install &amp; use git script</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Git Script are available at this place:
+http://www.vim.org/scripts/index.php
+Scripts are util and to install them, open e.g. supertab.vmb (this is the script file for supertab) with vim and type ":so %" at vim's command mode, then the installation is complete
+** fyi,supertab's page: http://www.vim.org/scripts/script.php?script_id=1643</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -462,7 +493,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -473,6 +504,15 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -581,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -608,9 +648,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -623,7 +670,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -697,6 +744,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -731,6 +779,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -906,461 +955,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="3" max="3" width="80.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>111</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
       <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>94</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
       <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>97</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
       <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
       <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="B16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="B32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="B33" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="B34" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="B44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="B45" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="B46" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="B47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="B48" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="B49" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3">
-      <c r="B50" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C7" s="14" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3">
-      <c r="B51" t="s">
-        <v>101</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3">
-      <c r="B52" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" ht="30">
-      <c r="B53" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1371,25 +1054,477 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add vim entry about visual selection
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
   <si>
     <t>Lang</t>
   </si>
@@ -460,16 +460,27 @@
 ** fyi,supertab's page: http://www.vim.org/scripts/script.php?script_id=1643</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>Visual</t>
+  </si>
+  <si>
+    <t>Visual Basic</t>
+  </si>
+  <si>
+    <t>V: select at line level
+v: select at char level
+Ctrl + v : select vertically at char level</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -493,7 +504,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -509,7 +520,7 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -657,7 +668,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -670,7 +681,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -744,7 +755,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -779,7 +789,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -955,21 +964,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="23.25" customWidth="1"/>
-    <col min="3" max="3" width="80.875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="80.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="16" t="s">
         <v>108</v>
       </c>
@@ -980,7 +989,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="90">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -991,7 +1000,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -1002,7 +1011,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -1044,6 +1053,17 @@
       </c>
       <c r="C7" s="14" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1054,21 +1074,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="26" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1090,7 +1110,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -1098,7 +1118,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -1106,7 +1126,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>37</v>
       </c>
@@ -1114,7 +1134,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="B6" t="s">
         <v>39</v>
       </c>
@@ -1122,7 +1142,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>41</v>
       </c>
@@ -1130,7 +1150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>43</v>
       </c>
@@ -1138,7 +1158,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="B9" t="s">
         <v>45</v>
       </c>
@@ -1146,7 +1166,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="B10" t="s">
         <v>47</v>
       </c>
@@ -1154,7 +1174,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>49</v>
       </c>
@@ -1162,7 +1182,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="B12" t="s">
         <v>51</v>
       </c>
@@ -1170,7 +1190,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="B13" t="s">
         <v>53</v>
       </c>
@@ -1178,7 +1198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>55</v>
       </c>
@@ -1186,7 +1206,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="B15" t="s">
         <v>57</v>
       </c>
@@ -1194,7 +1214,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="B16" t="s">
         <v>58</v>
       </c>
@@ -1202,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -1210,7 +1230,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
         <v>61</v>
       </c>
@@ -1218,7 +1238,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3">
       <c r="B19" t="s">
         <v>63</v>
       </c>
@@ -1226,7 +1246,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3">
       <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
@@ -1234,7 +1254,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
         <v>65</v>
       </c>
@@ -1242,7 +1262,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
         <v>68</v>
       </c>
@@ -1250,7 +1270,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
         <v>70</v>
       </c>
@@ -1258,7 +1278,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3">
       <c r="B24" t="s">
         <v>72</v>
       </c>
@@ -1266,7 +1286,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -1274,7 +1294,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3">
       <c r="B26" t="s">
         <v>76</v>
       </c>
@@ -1282,7 +1302,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3">
       <c r="B27" t="s">
         <v>78</v>
       </c>
@@ -1290,7 +1310,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
         <v>88</v>
       </c>
@@ -1298,7 +1318,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3">
       <c r="B29" t="s">
         <v>90</v>
       </c>
@@ -1306,7 +1326,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3">
       <c r="B30" t="s">
         <v>80</v>
       </c>
@@ -1314,7 +1334,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3">
       <c r="B31" t="s">
         <v>82</v>
       </c>
@@ -1322,7 +1342,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3">
       <c r="B32" t="s">
         <v>84</v>
       </c>
@@ -1330,7 +1350,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="B33" t="s">
         <v>86</v>
       </c>
@@ -1338,7 +1358,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="B34" t="s">
         <v>86</v>
       </c>
@@ -1346,7 +1366,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
         <v>4</v>
       </c>
@@ -1357,7 +1377,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" s="7"/>
       <c r="B36" s="8" t="s">
         <v>17</v>
@@ -1366,7 +1386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" s="7"/>
       <c r="B37" s="8" t="s">
         <v>19</v>
@@ -1375,7 +1395,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
         <v>21</v>
@@ -1384,7 +1404,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" s="7"/>
       <c r="B39" s="8" t="s">
         <v>23</v>
@@ -1393,7 +1413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" s="7"/>
       <c r="B40" s="8" t="s">
         <v>25</v>
@@ -1402,7 +1422,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" s="7"/>
       <c r="B41" s="8" t="s">
         <v>27</v>
@@ -1411,7 +1431,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3">
       <c r="A42" s="10"/>
       <c r="B42" s="11" t="s">
         <v>29</v>
@@ -1420,7 +1440,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1431,7 +1451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="B44" t="s">
         <v>9</v>
       </c>
@@ -1439,7 +1459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3">
       <c r="B45" t="s">
         <v>11</v>
       </c>
@@ -1447,7 +1467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="B46" t="s">
         <v>13</v>
       </c>
@@ -1455,7 +1475,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="B47" t="s">
         <v>94</v>
       </c>
@@ -1463,7 +1483,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3">
       <c r="B48" t="s">
         <v>97</v>
       </c>
@@ -1471,7 +1491,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3">
       <c r="B49" t="s">
         <v>96</v>
       </c>
@@ -1479,7 +1499,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3">
       <c r="B50" t="s">
         <v>98</v>
       </c>
@@ -1487,7 +1507,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3">
       <c r="B51" t="s">
         <v>101</v>
       </c>
@@ -1495,7 +1515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3">
       <c r="B52" s="3" t="s">
         <v>103</v>
       </c>
@@ -1503,7 +1523,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" ht="30">
       <c r="B53" t="s">
         <v>105</v>
       </c>
@@ -1519,12 +1539,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add entry on set vimrc tab to space & colorscheme
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="122">
   <si>
     <t>Lang</t>
   </si>
@@ -470,6 +470,26 @@
     <t>V: select at line level
 v: select at char level
 Ctrl + v : select vertically at char level</t>
+  </si>
+  <si>
+    <t>config</t>
+  </si>
+  <si>
+    <t>set tab to 4 spaces</t>
+  </si>
+  <si>
+    <t>set default colorscheme</t>
+  </si>
+  <si>
+    <t>In .vimrc, add:
+colorscheme darkblue      " myles put 2017-04-07 on set default colorscheme</t>
+  </si>
+  <si>
+    <t>In .vimrc, add:
+filetype plugin indent on       
+set tabstop=4                   "show existing tab with 4 spaces width
+set shiftwidth=4                " when indenting with '&gt;', use 4 spaces width
+set expandtab                   " On pressing tab, insert 4 spaces</t>
   </si>
 </sst>
 </file>
@@ -965,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1064,6 +1084,28 @@
       </c>
       <c r="C8" s="15" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add vim entry on search and substitile
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="128">
   <si>
     <t>Lang</t>
   </si>
@@ -491,16 +491,43 @@
 set shiftwidth=4                " when indenting with '&gt;', use 4 spaces width
 set expandtab                   " On pressing tab, insert 4 spaces</t>
   </si>
+  <si>
+    <t>replace</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Replace basic</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>search</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search basic</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>/keyword     //serach a keyword
+n               //search next hit
+N              //search last hit</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>:s/foo/bar/g          //do substitile in current line
+:%s/foo/bar/g       //do substitile in all lines</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -524,7 +551,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -540,7 +567,7 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -688,7 +715,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -701,7 +728,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -775,6 +802,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -809,6 +837,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -984,21 +1013,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="80.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="3" max="3" width="80.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>108</v>
       </c>
@@ -1009,7 +1038,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="90">
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -1020,7 +1049,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -1031,7 +1060,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -1042,7 +1071,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -1053,7 +1082,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -1064,7 +1093,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -1075,7 +1104,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -1086,7 +1115,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="75">
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -1097,7 +1126,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -1106,6 +1135,28 @@
       </c>
       <c r="C10" s="15" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1116,21 +1167,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="26" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" customHeight="1">
+    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1152,7 +1203,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -1160,7 +1211,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -1168,7 +1219,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>37</v>
       </c>
@@ -1176,7 +1227,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>39</v>
       </c>
@@ -1184,7 +1235,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>41</v>
       </c>
@@ -1192,7 +1243,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>43</v>
       </c>
@@ -1200,7 +1251,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>45</v>
       </c>
@@ -1208,7 +1259,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>47</v>
       </c>
@@ -1216,7 +1267,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>49</v>
       </c>
@@ -1224,7 +1275,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>51</v>
       </c>
@@ -1232,7 +1283,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>53</v>
       </c>
@@ -1240,7 +1291,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>55</v>
       </c>
@@ -1248,7 +1299,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>57</v>
       </c>
@@ -1256,7 +1307,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>58</v>
       </c>
@@ -1264,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -1272,7 +1323,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>61</v>
       </c>
@@ -1280,7 +1331,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>63</v>
       </c>
@@ -1288,7 +1339,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
@@ -1296,7 +1347,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>65</v>
       </c>
@@ -1304,7 +1355,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>68</v>
       </c>
@@ -1312,7 +1363,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>70</v>
       </c>
@@ -1320,7 +1371,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>72</v>
       </c>
@@ -1328,7 +1379,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -1336,7 +1387,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>76</v>
       </c>
@@ -1344,7 +1395,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>78</v>
       </c>
@@ -1352,7 +1403,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>88</v>
       </c>
@@ -1360,7 +1411,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>90</v>
       </c>
@@ -1368,7 +1419,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>80</v>
       </c>
@@ -1376,7 +1427,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>82</v>
       </c>
@@ -1384,7 +1435,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>84</v>
       </c>
@@ -1392,7 +1443,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>86</v>
       </c>
@@ -1400,7 +1451,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>86</v>
       </c>
@@ -1408,7 +1459,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>4</v>
       </c>
@@ -1419,7 +1470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="8" t="s">
         <v>17</v>
@@ -1428,7 +1479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="8" t="s">
         <v>19</v>
@@ -1437,7 +1488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
         <v>21</v>
@@ -1446,7 +1497,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="8" t="s">
         <v>23</v>
@@ -1455,7 +1506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="8" t="s">
         <v>25</v>
@@ -1464,7 +1515,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="8" t="s">
         <v>27</v>
@@ -1473,7 +1524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="11" t="s">
         <v>29</v>
@@ -1482,7 +1533,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1493,7 +1544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>9</v>
       </c>
@@ -1501,7 +1552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>11</v>
       </c>
@@ -1509,7 +1560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>13</v>
       </c>
@@ -1517,7 +1568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>94</v>
       </c>
@@ -1525,7 +1576,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>97</v>
       </c>
@@ -1533,7 +1584,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>96</v>
       </c>
@@ -1541,7 +1592,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>98</v>
       </c>
@@ -1549,7 +1600,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="2:3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>101</v>
       </c>
@@ -1557,7 +1608,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="2:3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
         <v>103</v>
       </c>
@@ -1565,7 +1616,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="30">
+    <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>105</v>
       </c>
@@ -1581,12 +1632,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Add how to type tab in vim 2. Add new Redis Library
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="134">
   <si>
     <t>Lang</t>
   </si>
@@ -454,13 +454,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Git Script are available at this place:
-http://www.vim.org/scripts/index.php
-Scripts are util and to install them, open e.g. supertab.vmb (this is the script file for supertab) with vim and type ":so %" at vim's command mode, then the installation is complete
-** fyi,supertab's page: http://www.vim.org/scripts/script.php?script_id=1643</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Visual</t>
   </si>
   <si>
@@ -527,6 +520,21 @@
   <si>
     <t>:set wrap
 :set nowrap</t>
+  </si>
+  <si>
+    <t>Git Script are available at this place:
+http://www.vim.org/scripts/index.php
+Scripts are util and to install them, open e.g. supertab.vmb (this is the script file for supertab) with vim and type ":so %" at vim's command mode, then the installation is complete
+** fyi,supertab's page: http://www.vim.org/scripts/script.php?script_id=1643</t>
+  </si>
+  <si>
+    <t>You can use &lt;CTRL-V&gt;&lt;Tab&gt; in "insert mode". In insert mode &lt;CTRL-V&gt; inserts a literal copy of your next character.</t>
+  </si>
+  <si>
+    <t>Insert &lt;Tab&gt; when expandtab ON</t>
+  </si>
+  <si>
+    <t>vim</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1054,7 +1062,7 @@
         <v>111</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1114,68 +1122,79 @@
     </row>
     <row r="8" spans="1:3" ht="45">
       <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
         <v>114</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="75">
       <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" t="s">
         <v>117</v>
       </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
       <c r="C9" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30">
       <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
         <v>122</v>
       </c>
-      <c r="B11" t="s">
-        <v>123</v>
-      </c>
       <c r="C11" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45">
       <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s">
         <v>124</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="15" t="s">
         <v>125</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30">
       <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" t="s">
         <v>128</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>130</v>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add vim entries on help, vimrc, fold, plugin etc
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="151">
   <si>
     <t>Lang</t>
   </si>
@@ -535,6 +535,70 @@
   </si>
   <si>
     <t>vim</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>The incsearch option allows sync search before the enter is press when type the /{keyowrd} command:
+:set incsearch</t>
+  </si>
+  <si>
+    <t>/{keyword} supports regular expression</t>
+  </si>
+  <si>
+    <t>:help 'option'
+In the help text, point the cursor to tag 'option' and go to tag with `Ctrl ]` to view all available options</t>
+  </si>
+  <si>
+    <t>~/.vimrc (personal config) overrides /etc/vimrc (general config)</t>
+  </si>
+  <si>
+    <t>fold</t>
+  </si>
+  <si>
+    <t>Set a fold:
+zf    (zf and then use search or visual before zf to determine the endpoint of folding)
+Open a fold:
+zo   (or l at the beginning of line)
+Close a fold:
+zc</t>
+  </si>
+  <si>
+    <t>vimrc override hierarchy</t>
+  </si>
+  <si>
+    <t>error fix</t>
+  </si>
+  <si>
+    <t>When use cygwin to run vim plugins, there are many error with ^M, it is because of the unix file format (end of line) is not align with windows'. The solution is change the target script's file format with vim with :set fileformat=unix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vim </t>
+  </si>
+  <si>
+    <t>edit multiple files</t>
+  </si>
+  <si>
+    <t>There are 3 ways to edit multiple files:
+1. Use split open
+2. Use tab open
+3. vim *.java
+For the vim *.java case, use :next / :n to move to next file</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>plugin manager- pathogen</t>
+  </si>
+  <si>
+    <t>The plugin manager pathogen:
+1. Installation: download the pathogen.vim to ~/.vim/autoload/pathogen.vim
+2. Usage: download any plugin into ~/.vim/bundle/ and pathogen will auto-deplay the plugin, so no need to change config file</t>
   </si>
 </sst>
 </file>
@@ -724,12 +788,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1030,24 +1096,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="80.85546875" customWidth="1"/>
+    <col min="3" max="3" width="80.85546875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>109</v>
       </c>
       <c r="C1" s="16" t="s">
@@ -1061,7 +1127,7 @@
       <c r="B2" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1127,7 +1193,7 @@
       <c r="B8" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1138,7 +1204,7 @@
       <c r="B9" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1149,7 +1215,7 @@
       <c r="B10" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1160,7 +1226,7 @@
       <c r="B11" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1171,7 +1237,7 @@
       <c r="B12" t="s">
         <v>124</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1182,19 +1248,115 @@
       <c r="B13" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" ht="30">
       <c r="A14" t="s">
         <v>133</v>
       </c>
       <c r="B14" t="s">
         <v>132</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="14" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45">
+      <c r="A16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="90">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="75">
+      <c r="A22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="60">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1208,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add config to vim
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -596,9 +596,11 @@
     <t>plugin manager- pathogen</t>
   </si>
   <si>
-    <t>The plugin manager pathogen:
-1. Installation: download the pathogen.vim to ~/.vim/autoload/pathogen.vim
-2. Usage: download any plugin into ~/.vim/bundle/ and pathogen will auto-deplay the plugin, so no need to change config file</t>
+    <t># The plugin manager pathogen:
+## Installation: 
+* download the pathogen.vim to ~/.vim/autoload/pathogen.vim
+* add to vimrc: execute pathogen#infect()
+## Usage: download any plugin into ~/.vim/bundle/ and pathogen will auto-deplay the plugin, so no need to change config file</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1101,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1348,7 +1350,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60">
+    <row r="23" spans="1:3" ht="90">
       <c r="A23" t="s">
         <v>133</v>
       </c>

</xml_diff>

<commit_message>
Add nerdtree cheatsheet and Add vim entry on nerdtree usage
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="154">
   <si>
     <t>Lang</t>
   </si>
@@ -601,6 +601,23 @@
 * download the pathogen.vim to ~/.vim/autoload/pathogen.vim
 * add to vimrc: execute pathogen#infect()
 ## Usage: download any plugin into ~/.vim/bundle/ and pathogen will auto-deplay the plugin, so no need to change config file</t>
+  </si>
+  <si>
+    <t>nerdtree</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t># Basic Ops
+o: open files
+t: open in tab
+i: open in split
+u: upper level of directory
+e: explore selected direcotry
+o/x: (de)select direcotry
+# How to open 
+:NERDTree {direcotry}</t>
   </si>
 </sst>
 </file>
@@ -1098,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1359,6 +1376,17 @@
       </c>
       <c r="C23" s="14" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="135">
+      <c r="A24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add how to fix cygwin vim nerdtree not working
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="156">
   <si>
     <t>Lang</t>
   </si>
@@ -618,6 +618,19 @@
 o/x: (de)select direcotry
 # How to open 
 :NERDTree {direcotry}</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
+    <t># Fix NERDTree not working on cygwin:
+* __Symptom__ when open file works but not able to open directory, And the expand/collapse arrow cannot show 
+* __Reason__ the failure of showing the arrow cause the direcotry select error
+* __Solution__ override the arrow charactor in vimrc by adding below lines:
+```
+let g:NERDTreeDirArrowExpandable="+"
+let g:NERDTreeDirArrowCollapsible="-"
+```</t>
   </si>
 </sst>
 </file>
@@ -1115,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1387,6 +1400,17 @@
       </c>
       <c r="C24" s="14" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="135">
+      <c r="A25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add vim entry on Syntastic and syntax folder
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="161">
   <si>
     <t>Lang</t>
   </si>
@@ -557,9 +557,6 @@
     <t>~/.vimrc (personal config) overrides /etc/vimrc (general config)</t>
   </si>
   <si>
-    <t>fold</t>
-  </si>
-  <si>
     <t>Set a fold:
 zf    (zf and then use search or visual before zf to determine the endpoint of folding)
 Open a fold:
@@ -607,17 +604,6 @@
   </si>
   <si>
     <t>basic</t>
-  </si>
-  <si>
-    <t># Basic Ops
-o: open files
-t: open in tab
-i: open in split
-u: upper level of directory
-e: explore selected direcotry
-o/x: (de)select direcotry
-# How to open 
-:NERDTree {direcotry}</t>
   </si>
   <si>
     <t>debug</t>
@@ -632,12 +618,70 @@
 let g:NERDTreeDirArrowCollapsible="-"
 ```</t>
   </si>
+  <si>
+    <t>fold (1)</t>
+  </si>
+  <si>
+    <t>fold (2)</t>
+  </si>
+  <si>
+    <t>Syntastic</t>
+  </si>
+  <si>
+    <t>NERDTree</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Basic Ops- file level
+o: open files
+t: open in tab
+i: open in split
+# Basic Ops- directory level
+u: upper level of directory
+e: explore selected direcotry
+o/x: (de)select direcotry
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O- open recursively</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+# How to open 
+:NERDTree {direcotry}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">:SyntasticCheck
+:SyntasticToggleMode   //I set this to vimrc when vim open, so that it turns Syntastic off </t>
+  </si>
+  <si>
+    <t>zR: Reduce the foldlevel to highest level so that all fold are expand
+zr: Reduce 1 from the foldlevel
+zM: More fold: set the foldlevel to 0
+zm: More 1 to the foldlevel
+:set foldlevel=n</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -684,6 +728,13 @@
       <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1128,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1308,7 +1359,7 @@
         <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>138</v>
@@ -1341,7 +1392,7 @@
         <v>133</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>139</v>
@@ -1352,10 +1403,10 @@
         <v>133</v>
       </c>
       <c r="B20" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45">
@@ -1363,21 +1414,21 @@
         <v>133</v>
       </c>
       <c r="B21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="75">
       <c r="A22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s">
         <v>145</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="14" t="s">
         <v>146</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="90">
@@ -1385,32 +1436,54 @@
         <v>133</v>
       </c>
       <c r="B23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="135">
+    </row>
+    <row r="24" spans="1:3" ht="165">
       <c r="A24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" t="s">
         <v>151</v>
       </c>
-      <c r="B24" t="s">
-        <v>152</v>
-      </c>
       <c r="C24" s="14" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="135">
       <c r="A25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="75">
+      <c r="A26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30">
+      <c r="A27" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" t="s">
         <v>151</v>
       </c>
-      <c r="B25" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>155</v>
+      <c r="C27" s="14" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add my vimrc snapshot
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="164">
   <si>
     <t>Lang</t>
   </si>
@@ -675,6 +675,51 @@
 zM: More fold: set the foldlevel to 0
 zm: More 1 to the foldlevel
 :set foldlevel=n</t>
+  </si>
+  <si>
+    <t>vimrc</t>
+  </si>
+  <si>
+    <t>snapshot</t>
+  </si>
+  <si>
+    <t>" myles put 2017-05-09 on indent tab to space
+filetype plugin indent on       
+set tabstop=4                   "show existing tab with 4 spaces width
+set shiftwidth=4                " when indenting with '&gt;', use 4 spaces width
+set expandtab                   " On pressing tab, insert 4 spaces
+" myles put 2017-05-09 on set default colorscheme
+colorscheme darkblue
+" Install pathogen 2017-05-23
+execute pathogen#infect()
+syntax on 
+" 2017-05-23 set option
+"set nowrap
+" 2017-05-24 set option
+set incsearch
+" 2017-05-24 Open Nerdtree when vim open with no input
+"autocmd StdinReadPre * let s:std_in=1
+"autocmd VimEnter * if argc() == 0 &amp;&amp; !exists("s:std_in") | NERDTree | endif
+" 2017-05-24 Create shortcut for NERDTree
+map &lt;C-n&gt; :NERDTreeToggle&lt;CR&gt;
+" 2017-05-25 Change the directory arrow
+let g:NERDTreeDirArrowExpandable="+"
+let g:NERDTreeDirArrowCollapsible="-"
+" 2017-05-25 Change the directory arrow
+autocmd BufWinLeave *.* mkview
+"autocmd BufWinEnter *.* silent loadview
+" 2017-05-25 Syntastic plugin 
+autocmd BufWinEnter *.* silent SyntasticToggleMode
+set statusline+=%#warningmsg#
+set statusline+=%{SyntasticStatuslineFlag()}
+set statusline+=%*
+let g:syntastic_always_populate_loc_list = 1
+let g:syntastic_auto_loc_list = 1
+"let g:syntastic_check_on_open = 1
+"let g:syntastic_check_on_wq = 0
+" 2017-05-26 Syntax folding autostart
+set foldmethod=syntax
+set foldlevel=1</t>
   </si>
 </sst>
 </file>
@@ -1179,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1484,6 +1529,17 @@
       </c>
       <c r="C27" s="14" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="92.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add vim entry about 3 types of vim plugin
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="167">
   <si>
     <t>Lang</t>
   </si>
@@ -646,7 +646,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -656,7 +656,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -720,17 +720,36 @@
 " 2017-05-26 Syntax folding autostart
 set foldmethod=syntax
 set foldlevel=1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>plugin</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Types of plugin</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t># 3 Types of vim plugin
+## single vim file
+This kind of standalone plugin can be installed by copy the file to .vim/plugin and reboot vim
+## vim bal (with fileextension vmb)
+Vim into the vmb file and :source % then the ball should provide script to install itself
+## A directory with sub folders
+This kind of vim plugin need plugin manager to install. Plugin manager pathogen I am using, or vundle, neobundle and etc</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -754,7 +773,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -770,7 +789,7 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -778,7 +797,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -927,7 +946,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -940,7 +959,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1014,6 +1033,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1048,6 +1068,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1223,21 +1244,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="80.85546875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="3" max="3" width="80.875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>108</v>
       </c>
@@ -1248,7 +1269,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="90">
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -1259,7 +1280,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -1270,7 +1291,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -1281,7 +1302,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -1292,7 +1313,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -1303,7 +1324,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -1314,7 +1335,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -1325,7 +1346,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="75">
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -1336,7 +1357,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -1347,7 +1368,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -1358,7 +1379,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -1369,7 +1390,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -1380,7 +1401,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1391,7 +1412,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -1399,7 +1420,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45">
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -1410,7 +1431,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>133</v>
       </c>
@@ -1421,7 +1442,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>133</v>
       </c>
@@ -1432,7 +1453,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>133</v>
       </c>
@@ -1443,7 +1464,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="90">
+    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -1454,7 +1475,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="45">
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -1465,7 +1486,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -1476,7 +1497,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="90">
+    <row r="23" spans="1:3" ht="90" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -1487,7 +1508,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="165">
+    <row r="24" spans="1:3" ht="165" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>157</v>
       </c>
@@ -1498,7 +1519,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="135">
+    <row r="25" spans="1:3" ht="135" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>150</v>
       </c>
@@ -1509,7 +1530,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="75">
+    <row r="26" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -1520,7 +1541,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -1531,7 +1552,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="92.25" customHeight="1">
+    <row r="28" spans="1:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>161</v>
       </c>
@@ -1540,6 +1561,17 @@
       </c>
       <c r="C28" s="14" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="135" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1550,21 +1582,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="26" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" customHeight="1">
+    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1618,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -1594,7 +1626,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -1602,7 +1634,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>37</v>
       </c>
@@ -1610,7 +1642,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>39</v>
       </c>
@@ -1618,7 +1650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>41</v>
       </c>
@@ -1626,7 +1658,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>43</v>
       </c>
@@ -1634,7 +1666,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>45</v>
       </c>
@@ -1642,7 +1674,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>47</v>
       </c>
@@ -1650,7 +1682,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>49</v>
       </c>
@@ -1658,7 +1690,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>51</v>
       </c>
@@ -1666,7 +1698,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>53</v>
       </c>
@@ -1674,7 +1706,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>55</v>
       </c>
@@ -1682,7 +1714,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>57</v>
       </c>
@@ -1690,7 +1722,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>58</v>
       </c>
@@ -1698,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -1706,7 +1738,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>61</v>
       </c>
@@ -1714,7 +1746,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>63</v>
       </c>
@@ -1722,7 +1754,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
@@ -1730,7 +1762,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>65</v>
       </c>
@@ -1738,7 +1770,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>68</v>
       </c>
@@ -1746,7 +1778,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>70</v>
       </c>
@@ -1754,7 +1786,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>72</v>
       </c>
@@ -1762,7 +1794,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -1770,7 +1802,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>76</v>
       </c>
@@ -1778,7 +1810,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>78</v>
       </c>
@@ -1786,7 +1818,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>88</v>
       </c>
@@ -1794,7 +1826,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>90</v>
       </c>
@@ -1802,7 +1834,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>80</v>
       </c>
@@ -1810,7 +1842,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>82</v>
       </c>
@@ -1818,7 +1850,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>84</v>
       </c>
@@ -1826,7 +1858,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>86</v>
       </c>
@@ -1834,7 +1866,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>86</v>
       </c>
@@ -1842,7 +1874,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>4</v>
       </c>
@@ -1853,7 +1885,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="8" t="s">
         <v>17</v>
@@ -1862,7 +1894,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="8" t="s">
         <v>19</v>
@@ -1871,7 +1903,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
         <v>21</v>
@@ -1880,7 +1912,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="8" t="s">
         <v>23</v>
@@ -1889,7 +1921,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="8" t="s">
         <v>25</v>
@@ -1898,7 +1930,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="8" t="s">
         <v>27</v>
@@ -1907,7 +1939,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="11" t="s">
         <v>29</v>
@@ -1916,7 +1948,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1927,7 +1959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>9</v>
       </c>
@@ -1935,7 +1967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>11</v>
       </c>
@@ -1943,7 +1975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>13</v>
       </c>
@@ -1951,7 +1983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>94</v>
       </c>
@@ -1959,7 +1991,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>97</v>
       </c>
@@ -1967,7 +1999,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>96</v>
       </c>
@@ -1975,7 +2007,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>98</v>
       </c>
@@ -1983,7 +2015,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="2:3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>101</v>
       </c>
@@ -1991,7 +2023,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="2:3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
         <v>103</v>
       </c>
@@ -1999,7 +2031,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="30">
+    <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>105</v>
       </c>
@@ -2015,12 +2047,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add vim entry on Macro!
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="170">
   <si>
     <t>Lang</t>
   </si>
@@ -646,7 +646,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -656,7 +656,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -740,16 +740,31 @@
 This kind of vim plugin need plugin manager to install. Plugin manager pathogen I am using, or vundle, neobundle and etc</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>macro</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t># Intro to Macro
+Vim macro is a record &amp; paly procedure.
+# Example
+* Start recording: `qa` (q means start recording and a is the macro name)
+* do sth. (when recording the status bar shows the word)
+* Stop recording: `q`
+* Invoke the macro: `5@a` (means perform the a macro from current line for 5 times)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -773,7 +788,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -789,7 +804,7 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -797,7 +812,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -946,7 +961,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -959,7 +974,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1033,7 +1048,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1068,7 +1082,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1244,21 +1257,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="23.25" customWidth="1"/>
-    <col min="3" max="3" width="80.875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="80.85546875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="15" t="s">
         <v>108</v>
       </c>
@@ -1269,7 +1282,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="90">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -1280,7 +1293,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -1291,7 +1304,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -1302,7 +1315,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -1313,7 +1326,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -1324,7 +1337,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -1335,7 +1348,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -1346,7 +1359,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="75">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -1357,7 +1370,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -1368,7 +1381,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -1379,7 +1392,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="45">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -1390,7 +1403,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="30">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -1401,7 +1414,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="30">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1412,7 +1425,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -1420,7 +1433,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="45">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -1431,7 +1444,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>133</v>
       </c>
@@ -1442,7 +1455,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>133</v>
       </c>
@@ -1453,7 +1466,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>133</v>
       </c>
@@ -1464,7 +1477,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="90">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -1475,7 +1488,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="45">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -1486,7 +1499,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="75">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -1497,7 +1510,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="90" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="90">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -1508,7 +1521,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="165" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="165">
       <c r="A24" t="s">
         <v>157</v>
       </c>
@@ -1519,7 +1532,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="135" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="135">
       <c r="A25" t="s">
         <v>150</v>
       </c>
@@ -1530,7 +1543,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="75">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -1541,7 +1554,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="30">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -1552,7 +1565,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="92.25" customHeight="1">
       <c r="A28" t="s">
         <v>161</v>
       </c>
@@ -1563,7 +1576,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="135" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="135">
       <c r="A29" t="s">
         <v>164</v>
       </c>
@@ -1572,6 +1585,17 @@
       </c>
       <c r="C29" s="14" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="105">
+      <c r="A30" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1582,21 +1606,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="26" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1607,7 +1631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1618,7 +1642,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -1626,7 +1650,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -1634,7 +1658,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>37</v>
       </c>
@@ -1642,7 +1666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="B6" t="s">
         <v>39</v>
       </c>
@@ -1650,7 +1674,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>41</v>
       </c>
@@ -1658,7 +1682,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>43</v>
       </c>
@@ -1666,7 +1690,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="B9" t="s">
         <v>45</v>
       </c>
@@ -1674,7 +1698,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="B10" t="s">
         <v>47</v>
       </c>
@@ -1682,7 +1706,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>49</v>
       </c>
@@ -1690,7 +1714,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="B12" t="s">
         <v>51</v>
       </c>
@@ -1698,7 +1722,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="B13" t="s">
         <v>53</v>
       </c>
@@ -1706,7 +1730,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>55</v>
       </c>
@@ -1714,7 +1738,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="B15" t="s">
         <v>57</v>
       </c>
@@ -1722,7 +1746,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="B16" t="s">
         <v>58</v>
       </c>
@@ -1730,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -1738,7 +1762,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
         <v>61</v>
       </c>
@@ -1746,7 +1770,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3">
       <c r="B19" t="s">
         <v>63</v>
       </c>
@@ -1754,7 +1778,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3">
       <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
@@ -1762,7 +1786,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
         <v>65</v>
       </c>
@@ -1770,7 +1794,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
         <v>68</v>
       </c>
@@ -1778,7 +1802,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
         <v>70</v>
       </c>
@@ -1786,7 +1810,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3">
       <c r="B24" t="s">
         <v>72</v>
       </c>
@@ -1794,7 +1818,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -1802,7 +1826,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3">
       <c r="B26" t="s">
         <v>76</v>
       </c>
@@ -1810,7 +1834,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3">
       <c r="B27" t="s">
         <v>78</v>
       </c>
@@ -1818,7 +1842,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
         <v>88</v>
       </c>
@@ -1826,7 +1850,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3">
       <c r="B29" t="s">
         <v>90</v>
       </c>
@@ -1834,7 +1858,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3">
       <c r="B30" t="s">
         <v>80</v>
       </c>
@@ -1842,7 +1866,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3">
       <c r="B31" t="s">
         <v>82</v>
       </c>
@@ -1850,7 +1874,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3">
       <c r="B32" t="s">
         <v>84</v>
       </c>
@@ -1858,7 +1882,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="B33" t="s">
         <v>86</v>
       </c>
@@ -1866,7 +1890,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="B34" t="s">
         <v>86</v>
       </c>
@@ -1874,7 +1898,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
         <v>4</v>
       </c>
@@ -1885,7 +1909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" s="7"/>
       <c r="B36" s="8" t="s">
         <v>17</v>
@@ -1894,7 +1918,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" s="7"/>
       <c r="B37" s="8" t="s">
         <v>19</v>
@@ -1903,7 +1927,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
         <v>21</v>
@@ -1912,7 +1936,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" s="7"/>
       <c r="B39" s="8" t="s">
         <v>23</v>
@@ -1921,7 +1945,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" s="7"/>
       <c r="B40" s="8" t="s">
         <v>25</v>
@@ -1930,7 +1954,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" s="7"/>
       <c r="B41" s="8" t="s">
         <v>27</v>
@@ -1939,7 +1963,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3">
       <c r="A42" s="10"/>
       <c r="B42" s="11" t="s">
         <v>29</v>
@@ -1948,7 +1972,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1959,7 +1983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="B44" t="s">
         <v>9</v>
       </c>
@@ -1967,7 +1991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3">
       <c r="B45" t="s">
         <v>11</v>
       </c>
@@ -1975,7 +1999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="B46" t="s">
         <v>13</v>
       </c>
@@ -1983,7 +2007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="B47" t="s">
         <v>94</v>
       </c>
@@ -1991,7 +2015,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3">
       <c r="B48" t="s">
         <v>97</v>
       </c>
@@ -1999,7 +2023,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3">
       <c r="B49" t="s">
         <v>96</v>
       </c>
@@ -2007,7 +2031,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3">
       <c r="B50" t="s">
         <v>98</v>
       </c>
@@ -2015,7 +2039,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3">
       <c r="B51" t="s">
         <v>101</v>
       </c>
@@ -2023,7 +2047,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3">
       <c r="B52" s="3" t="s">
         <v>103</v>
       </c>
@@ -2031,7 +2055,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" ht="30">
       <c r="B53" t="s">
         <v>105</v>
       </c>
@@ -2047,12 +2071,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add vim entry on function listing plugin Tagbar
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="173">
   <si>
     <t>Lang</t>
   </si>
@@ -754,6 +754,18 @@
 * do sth. (when recording the status bar shows the word)
 * Stop recording: `q`
 * Invoke the macro: `5@a` (means perform the a macro from current line for 5 times)</t>
+  </si>
+  <si>
+    <t>Tagbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A plugin to list functions </t>
+  </si>
+  <si>
+    <t># Download and install with Pathogen
+Navigate to .vim/bundle and download: https://github.com/majutsushi/tagbar
+# Prequisition
+Ctags, util that can be installed with dpkg/ apt-get/ apt-cyg</t>
   </si>
 </sst>
 </file>
@@ -1258,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1596,6 +1608,17 @@
       </c>
       <c r="C30" s="14" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="60">
+      <c r="A31" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add vim entry on markdown support in tagbar & vimrc snapshot
</commit_message>
<xml_diff>
--- a/vim_lib.xlsx
+++ b/vim_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="176">
   <si>
     <t>Lang</t>
   </si>
@@ -680,7 +680,49 @@
     <t>vimrc</t>
   </si>
   <si>
-    <t>snapshot</t>
+    <t>plugin</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Types of plugin</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t># 3 Types of vim plugin
+## single vim file
+This kind of standalone plugin can be installed by copy the file to .vim/plugin and reboot vim
+## vim bal (with fileextension vmb)
+Vim into the vmb file and :source % then the ball should provide script to install itself
+## A directory with sub folders
+This kind of vim plugin need plugin manager to install. Plugin manager pathogen I am using, or vundle, neobundle and etc</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>macro</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t># Intro to Macro
+Vim macro is a record &amp; paly procedure.
+# Example
+* Start recording: `qa` (q means start recording and a is the macro name)
+* do sth. (when recording the status bar shows the word)
+* Stop recording: `q`
+* Invoke the macro: `5@a` (means perform the a macro from current line for 5 times)</t>
+  </si>
+  <si>
+    <t>Tagbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A plugin to list functions </t>
+  </si>
+  <si>
+    <t># Download and install with Pathogen
+Navigate to .vim/bundle and download: https://github.com/majutsushi/tagbar
+# Prequisition
+Ctags, util that can be installed with dpkg/ apt-get/ apt-cyg</t>
   </si>
   <si>
     <t>" myles put 2017-05-09 on indent tab to space
@@ -720,52 +762,90 @@
 " 2017-05-26 Syntax folding autostart
 set foldmethod=syntax
 set foldlevel=1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>plugin</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Types of plugin</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t># 3 Types of vim plugin
-## single vim file
-This kind of standalone plugin can be installed by copy the file to .vim/plugin and reboot vim
-## vim bal (with fileextension vmb)
-Vim into the vmb file and :source % then the ball should provide script to install itself
-## A directory with sub folders
-This kind of vim plugin need plugin manager to install. Plugin manager pathogen I am using, or vundle, neobundle and etc</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>macro</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t># Intro to Macro
-Vim macro is a record &amp; paly procedure.
-# Example
-* Start recording: `qa` (q means start recording and a is the macro name)
-* do sth. (when recording the status bar shows the word)
-* Stop recording: `q`
-* Invoke the macro: `5@a` (means perform the a macro from current line for 5 times)</t>
-  </si>
-  <si>
-    <t>Tagbar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A plugin to list functions </t>
-  </si>
-  <si>
-    <t># Download and install with Pathogen
-Navigate to .vim/bundle and download: https://github.com/majutsushi/tagbar
-# Prequisition
-Ctags, util that can be installed with dpkg/ apt-get/ apt-cyg</t>
+  </si>
+  <si>
+    <t>snapshot/ 20170526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">" myles put 2017-05-09 on indent tab to space
+filetype plugin indent on
+set tabstop=4                   "show existing tab with 4 spaces width
+set shiftwidth=4                " when indenting with '&gt;', use 4 spaces width
+set expandtab                   " On pressing tab, insert 4 spaces
+" myles put 2017-05-09 on set default colorscheme
+colorscheme elflord
+" Install pathogen 2017-05-23
+execute pathogen#infect()
+syntax on
+" 2017-05-23 set option
+"set nowrap
+" 2017-05-24 set option
+set incsearch
+set hlsearch
+" 2017-05-24 Open Nerdtree when vim open with no input
+"autocmd StdinReadPre * let s:std_in=1
+"autocmd VimEnter * if argc() == 0 &amp;&amp; !exists("s:std_in") | NERDTree | endif
+" 2017-05-24 Create shortcut for NERDTree
+map &lt;C-n&gt; :NERDTreeToggle&lt;CR&gt;
+" 2017-05-25 Change the directory arrow
+let g:NERDTreeDirArrowExpandable="+"
+let g:NERDTreeDirArrowCollapsible="-"
+" 2017-05-25 Change the directory arrow
+autocmd BufWinLeave *.* mkview
+"autocmd BufWinEnter *.* silent loadview
+" 2017-05-25 Syntastic plugin
+" autocmd BufWinEnter *.* silent SyntasticToggleMode
+" set statusline+=%#warningmsg#
+" set statusline+=%{SyntasticStatuslineFlag()}
+" set statusline+=%*
+" let g:syntastic_always_populate_loc_list = 1
+" let g:syntastic_auto_loc_list = 1
+" let g:syntastic_check_on_open = 1
+" let g:syntastic_check_on_wq = 0
+" 2017-05-26 Syntax folding autostart
+set foldmethod=syntax
+set foldlevel=1
+" 2017-06-13 Shortcut for Tagbar/ learnt that &lt;ENTER&gt; also bind to map
+map &lt;C-m&gt; :TagbarToggle&lt;CR&gt;
+" 2017-06-26 Add support for markdown files in tagbar.
+let g:tagbar_type_markdown = {
+    \ 'ctagstype': 'markdown',
+    \ 'ctagsbin' : '~/.vim/support-script/markdown2ctags/markdown2ctags.py',
+    \ 'ctagsargs' : '-f - --sort=yes',
+    \ 'kinds' : [
+        \ 's:sections',
+        \ 'i:images'
+    \ ],
+    \ 'sro' : '|',
+    \ 'kind2scope' : {
+        \ 's' : 'section',
+    \ },
+    \ 'sort': 0,
+\ }
+</t>
+  </si>
+  <si>
+    <t>Add markdown support</t>
+  </si>
+  <si>
+    <t># Add markdown support for tagbar
+1. download https://github.com/jszakmeister/markdown2ctags to somewhere.
+1. add below snippet to .vimrc:
+" Add support for markdown files in tagbar.
+let g:tagbar_type_markdown = {
+    \ 'ctagstype': 'markdown',
+    \ 'ctagsbin' : '/path/to/markdown2ctags.py',
+    \ 'ctagsargs' : '-f - --sort=yes',
+    \ 'kinds' : [
+        \ 's:sections',
+        \ 'i:images'
+    \ ],
+    \ 'sro' : '|',
+    \ 'kind2scope' : {
+        \ 's' : 'section',
+    \ },
+    \ 'sort': 0,
+\ }</t>
   </si>
 </sst>
 </file>
@@ -1270,9 +1350,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -1582,43 +1662,65 @@
         <v>161</v>
       </c>
       <c r="B28" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="135">
       <c r="A29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>164</v>
-      </c>
-      <c r="B29" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="105">
       <c r="A30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="B30" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="60">
       <c r="A31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B31" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" s="14" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="95.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="101.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" t="s">
         <v>172</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>